<commit_message>
second commit -- uploading finished analysis
</commit_message>
<xml_diff>
--- a/in-depth-pitch/raw-data/clt-database.xlsx
+++ b/in-depth-pitch/raw-data/clt-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisa/dataProjects/in-depth-pitch/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FAA6F3-36B5-0944-A5EE-6C306829D976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2C9DDA-6ED1-F643-A06F-962B108F70C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16940" xr2:uid="{3CC013F5-54C7-8549-BFDA-D55347608270}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$19</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -183,12 +186,6 @@
     <t>https://ehebclt.nyc/</t>
   </si>
   <si>
-    <t xml:space="preserve">Has land? </t>
-  </si>
-  <si>
-    <t>Has buildings?</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
   </si>
   <si>
     <t>Inactive</t>
-  </si>
-  <si>
-    <t>1980s</t>
   </si>
   <si>
     <t>16 2nd Ave New York City, NY 10003 United States</t>
@@ -366,22 +360,19 @@
     <t>Redline rating</t>
   </si>
   <si>
-    <t xml:space="preserve">D </t>
-  </si>
-  <si>
     <t>A/B</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>D/not rated</t>
-  </si>
-  <si>
-    <t>C/not rated</t>
-  </si>
-  <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Has land</t>
+  </si>
+  <si>
+    <t>Has buildings</t>
   </si>
 </sst>
 </file>
@@ -809,7 +800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K19" sqref="K19"/>
+      <selection pane="topRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,7 +817,7 @@
         <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -835,32 +826,32 @@
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="6">
         <v>10302</v>
@@ -881,19 +872,19 @@
         <v>2022</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -903,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -919,19 +910,19 @@
         <v>2021</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -944,34 +935,34 @@
         <v>11212</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G4" s="5">
         <v>2018</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N4" s="5"/>
     </row>
@@ -983,10 +974,10 @@
         <v>11210</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>41</v>
@@ -998,19 +989,19 @@
         <v>2020</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -1023,7 +1014,7 @@
         <v>10038</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>16</v>
@@ -1032,25 +1023,25 @@
         <v>43</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="5">
         <v>2021</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -1060,37 +1051,37 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G7" s="5">
         <v>2018</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -1100,37 +1091,37 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G8" s="5">
         <v>1994</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -1143,34 +1134,34 @@
         <v>10009</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>58</v>
+        <v>80</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1980</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
@@ -1183,34 +1174,34 @@
         <v>10003</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G10" s="5">
         <v>2020</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -1238,19 +1229,19 @@
         <v>2014</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -1272,25 +1263,25 @@
         <v>31</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G12" s="5">
         <v>2017</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
@@ -1303,7 +1294,7 @@
         <v>10460</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>32</v>
@@ -1318,19 +1309,19 @@
         <v>2018</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1340,37 +1331,37 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G14" s="5">
         <v>2018</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
@@ -1383,7 +1374,7 @@
         <v>10468</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>20</v>
@@ -1392,25 +1383,25 @@
         <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G15" s="5">
         <v>2018</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
@@ -1423,7 +1414,7 @@
         <v>10454</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>19</v>
@@ -1432,25 +1423,25 @@
         <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G16" s="5">
         <v>2014</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
@@ -1470,25 +1461,25 @@
         <v>38</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G17" s="5">
         <v>2019</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -1501,34 +1492,34 @@
         <v>11372</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G18" s="5">
         <v>2018</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -1556,19 +1547,19 @@
         <v>2020</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -1580,6 +1571,7 @@
       <c r="A22" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N19" xr:uid="{08F68F1E-C361-5F4E-A854-EB63E3694F89}"/>
   <hyperlinks>
     <hyperlink ref="J9" r:id="rId1" xr:uid="{ABB82AEF-3ECB-494B-AA59-5078E44FE7CD}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{4D1F99A5-B51D-564D-B8EB-FD8FBCAF5277}"/>
@@ -1602,7 +1594,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -1612,7 +1604,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>